<commit_message>
Download Holiday Template Fix
</commit_message>
<xml_diff>
--- a/template/HolidayTemplate.xlsx
+++ b/template/HolidayTemplate.xlsx
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Holiday Name</t>
   </si>
@@ -140,9 +140,6 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>TAMIL PONGAL</t>
-  </si>
-  <si>
     <t>Asia/Kolkata</t>
   </si>
   <si>
@@ -150,6 +147,18 @@
   </si>
   <si>
     <t>Chennai</t>
+  </si>
+  <si>
+    <t>BHOGI PONGAL</t>
+  </si>
+  <si>
+    <t>THAI PONGAL</t>
+  </si>
+  <si>
+    <t>MATTU PONGAL</t>
+  </si>
+  <si>
+    <t>KANNUM PONGAL</t>
   </si>
 </sst>
 </file>
@@ -157,7 +166,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-14009]yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -236,9 +245,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -538,7 +547,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C21:C22"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" thickBottom="1"/>
@@ -576,10 +585,10 @@
     </row>
     <row r="2" spans="1:7" thickBot="1">
       <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="8">
         <v>45305</v>
@@ -591,18 +600,18 @@
         <v>2024</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" thickBot="1">
       <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="7">
         <v>45306</v>
@@ -614,18 +623,18 @@
         <v>2024</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" thickBot="1">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="7">
         <v>45307</v>
@@ -637,18 +646,18 @@
         <v>2024</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" thickBot="1">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="7">
         <v>45308</v>
@@ -660,10 +669,10 @@
         <v>2024</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>